<commit_message>
09/07/2024 fin de journée SCB
</commit_message>
<xml_diff>
--- a/tests/fichier_test/fp_compare.xlsx
+++ b/tests/fichier_test/fp_compare.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projet SCB\Project\reHabi\tests\fichier_test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Feuil1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2468" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2474" uniqueCount="433">
   <si>
     <t>nom</t>
   </si>
@@ -1318,8 +1323,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1376,58 +1380,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1438,10 +1445,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1479,71 +1486,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1571,7 +1578,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1594,11 +1601,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1607,13 +1614,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1623,7 +1630,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1632,7 +1639,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1641,7 +1648,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1649,10 +1656,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1723,33 +1730,35 @@
   </sheetPr>
   <dimension ref="A1:T136"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="39.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="22.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="11" width="28.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="13" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="11" width="26.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="14" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="11" width="19.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="11" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="11" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="11" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="11" width="23.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.140625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1811,7 +1820,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -1827,7 +1836,9 @@
       <c r="E2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1869,7 +1880,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="3" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1885,7 +1896,9 @@
       <c r="E3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
@@ -1927,7 +1940,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="4" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1943,7 +1956,9 @@
       <c r="E4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1985,7 +2000,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2001,7 +2016,9 @@
       <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
@@ -2043,7 +2060,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -2059,7 +2076,9 @@
       <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G6" s="2" t="s">
         <v>25</v>
       </c>
@@ -2101,7 +2120,7 @@
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="7" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -2117,7 +2136,9 @@
       <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2159,7 +2180,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="8" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2219,7 +2240,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -2277,7 +2298,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="10" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>76</v>
       </c>
@@ -2337,7 +2358,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="11" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>76</v>
       </c>
@@ -2397,7 +2418,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="12" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>76</v>
       </c>
@@ -2457,7 +2478,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="13" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>76</v>
       </c>
@@ -2517,7 +2538,7 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="14" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>76</v>
       </c>
@@ -2577,7 +2598,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="15" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>76</v>
       </c>
@@ -2637,7 +2658,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="16" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>76</v>
       </c>
@@ -2697,7 +2718,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="17" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>100</v>
       </c>
@@ -2755,7 +2776,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="18" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>100</v>
       </c>
@@ -2813,7 +2834,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="19" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>100</v>
       </c>
@@ -2871,7 +2892,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="20" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>100</v>
       </c>
@@ -2929,7 +2950,7 @@
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="21" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -2987,7 +3008,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="22" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>118</v>
       </c>
@@ -3045,7 +3066,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="23" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>124</v>
       </c>
@@ -3103,7 +3124,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="24" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>124</v>
       </c>
@@ -3161,7 +3182,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="25" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>124</v>
       </c>
@@ -3219,7 +3240,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="26" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>124</v>
       </c>
@@ -3277,7 +3298,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="27" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>124</v>
       </c>
@@ -3335,7 +3356,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="28" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>124</v>
       </c>
@@ -3393,7 +3414,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="29" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>124</v>
       </c>
@@ -3451,7 +3472,7 @@
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="30" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>124</v>
       </c>
@@ -3509,7 +3530,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="31" spans="1:20" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>130</v>
       </c>
@@ -3567,7 +3588,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="32" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>130</v>
       </c>
@@ -3625,7 +3646,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="33" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>135</v>
       </c>
@@ -3683,7 +3704,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="34" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>135</v>
       </c>
@@ -3741,7 +3762,7 @@
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="35" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>140</v>
       </c>
@@ -3799,7 +3820,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="36" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>140</v>
       </c>
@@ -3857,7 +3878,7 @@
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="37" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>143</v>
       </c>
@@ -3915,7 +3936,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="38" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>143</v>
       </c>
@@ -3973,7 +3994,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="39" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>143</v>
       </c>
@@ -4031,7 +4052,7 @@
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="40" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>143</v>
       </c>
@@ -4089,7 +4110,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="41" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>154</v>
       </c>
@@ -4147,7 +4168,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="42" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>154</v>
       </c>
@@ -4205,7 +4226,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="43" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>154</v>
       </c>
@@ -4263,7 +4284,7 @@
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="44" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>154</v>
       </c>
@@ -4321,7 +4342,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="45" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>163</v>
       </c>
@@ -4379,7 +4400,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="46" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>163</v>
       </c>
@@ -4437,7 +4458,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="47" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>163</v>
       </c>
@@ -4495,7 +4516,7 @@
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="48" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>163</v>
       </c>
@@ -4553,7 +4574,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="49" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>175</v>
       </c>
@@ -4611,7 +4632,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="50" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>175</v>
       </c>
@@ -4669,7 +4690,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="51" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>175</v>
       </c>
@@ -4727,7 +4748,7 @@
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="52" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>175</v>
       </c>
@@ -4785,7 +4806,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="53" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>178</v>
       </c>
@@ -4843,7 +4864,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="54" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>178</v>
       </c>
@@ -4901,7 +4922,7 @@
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="55" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>181</v>
       </c>
@@ -4959,7 +4980,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="56" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>181</v>
       </c>
@@ -5017,7 +5038,7 @@
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="57" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>185</v>
       </c>
@@ -5075,7 +5096,7 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="58" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>188</v>
       </c>
@@ -5133,7 +5154,7 @@
         <v>194</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="59" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>188</v>
       </c>
@@ -5191,7 +5212,7 @@
         <v>198</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="60" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>199</v>
       </c>
@@ -5251,7 +5272,7 @@
         <v>194</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="61" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>199</v>
       </c>
@@ -5311,7 +5332,7 @@
         <v>198</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="62" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>203</v>
       </c>
@@ -5369,7 +5390,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="63" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>203</v>
       </c>
@@ -5427,7 +5448,7 @@
         <v>214</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="64" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>203</v>
       </c>
@@ -5485,7 +5506,7 @@
         <v>217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="65" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>219</v>
       </c>
@@ -5543,7 +5564,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="66" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>219</v>
       </c>
@@ -5601,7 +5622,7 @@
         <v>214</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="67" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>219</v>
       </c>
@@ -5659,7 +5680,7 @@
         <v>217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="68" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>222</v>
       </c>
@@ -5717,7 +5738,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="69" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>222</v>
       </c>
@@ -5775,7 +5796,7 @@
         <v>214</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="70" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>222</v>
       </c>
@@ -5833,7 +5854,7 @@
         <v>217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="71" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>222</v>
       </c>
@@ -5891,7 +5912,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="72" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>222</v>
       </c>
@@ -5949,7 +5970,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="73" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>227</v>
       </c>
@@ -6007,7 +6028,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="74" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>227</v>
       </c>
@@ -6065,7 +6086,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="75" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>230</v>
       </c>
@@ -6123,7 +6144,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="76" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>230</v>
       </c>
@@ -6181,7 +6202,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="77" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>233</v>
       </c>
@@ -6239,7 +6260,7 @@
         <v>243</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="78" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>233</v>
       </c>
@@ -6297,7 +6318,7 @@
         <v>245</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="79" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>247</v>
       </c>
@@ -6355,7 +6376,7 @@
         <v>243</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="80" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>247</v>
       </c>
@@ -6413,7 +6434,7 @@
         <v>245</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="81" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>247</v>
       </c>
@@ -6471,7 +6492,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="82" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>251</v>
       </c>
@@ -6529,7 +6550,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="83" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>251</v>
       </c>
@@ -6587,7 +6608,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="84" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>257</v>
       </c>
@@ -6645,7 +6666,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="85" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>257</v>
       </c>
@@ -6703,7 +6724,7 @@
         <v>261</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="86" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>262</v>
       </c>
@@ -6761,7 +6782,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="87" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>262</v>
       </c>
@@ -6819,7 +6840,7 @@
         <v>261</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="88" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>269</v>
       </c>
@@ -6877,7 +6898,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="89" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>269</v>
       </c>
@@ -6935,7 +6956,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="90" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>277</v>
       </c>
@@ -6995,7 +7016,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="91" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>277</v>
       </c>
@@ -7055,7 +7076,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="92" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>277</v>
       </c>
@@ -7115,7 +7136,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="93" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>277</v>
       </c>
@@ -7175,7 +7196,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="94" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>277</v>
       </c>
@@ -7235,7 +7256,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="95" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>277</v>
       </c>
@@ -7295,7 +7316,7 @@
         <v>287</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="96" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>288</v>
       </c>
@@ -7353,7 +7374,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="97" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>288</v>
       </c>
@@ -7411,7 +7432,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="98" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>296</v>
       </c>
@@ -7469,7 +7490,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="99" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>296</v>
       </c>
@@ -7527,7 +7548,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="100" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>300</v>
       </c>
@@ -7585,7 +7606,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="101" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>305</v>
       </c>
@@ -7643,7 +7664,7 @@
         <v>311</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="102" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>312</v>
       </c>
@@ -7701,7 +7722,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="103" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>318</v>
       </c>
@@ -7759,7 +7780,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="104" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>324</v>
       </c>
@@ -7817,7 +7838,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="105" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>328</v>
       </c>
@@ -7875,7 +7896,7 @@
         <v>287</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="106" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>328</v>
       </c>
@@ -7933,7 +7954,7 @@
         <v>287</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="107" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>333</v>
       </c>
@@ -7991,7 +8012,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="108" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>339</v>
       </c>
@@ -8049,7 +8070,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="109" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>344</v>
       </c>
@@ -8107,7 +8128,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="33" customFormat="1" s="1">
+    <row r="110" spans="1:20" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>350</v>
       </c>
@@ -8165,7 +8186,7 @@
         <v>358</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="111" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>350</v>
       </c>
@@ -8223,7 +8244,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="112" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>360</v>
       </c>
@@ -8281,7 +8302,7 @@
         <v>311</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="113" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>366</v>
       </c>
@@ -8339,7 +8360,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="114" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>366</v>
       </c>
@@ -8397,7 +8418,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="115" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>366</v>
       </c>
@@ -8455,7 +8476,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="116" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>366</v>
       </c>
@@ -8513,7 +8534,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="117" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>371</v>
       </c>
@@ -8571,7 +8592,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="118" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>376</v>
       </c>
@@ -8629,7 +8650,7 @@
         <v>287</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="119" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>376</v>
       </c>
@@ -8687,7 +8708,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="120" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>380</v>
       </c>
@@ -8745,7 +8766,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="121" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>385</v>
       </c>
@@ -8803,7 +8824,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="122" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>390</v>
       </c>
@@ -8861,7 +8882,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="123" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>390</v>
       </c>
@@ -8919,7 +8940,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="124" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>390</v>
       </c>
@@ -8977,7 +8998,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="125" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>390</v>
       </c>
@@ -9035,7 +9056,7 @@
         <v>287</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="126" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>394</v>
       </c>
@@ -9093,7 +9114,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
+    <row r="127" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>399</v>
       </c>
@@ -9151,7 +9172,7 @@
         <v>311</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
+    <row r="128" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>405</v>
       </c>
@@ -9209,7 +9230,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
+    <row r="129" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>405</v>
       </c>
@@ -9267,7 +9288,7 @@
         <v>194</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
+    <row r="130" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>405</v>
       </c>
@@ -9325,7 +9346,7 @@
         <v>198</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
+    <row r="131" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>405</v>
       </c>
@@ -9383,7 +9404,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
+    <row r="132" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>405</v>
       </c>
@@ -9441,7 +9462,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="133" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>410</v>
       </c>
@@ -9501,7 +9522,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="134" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>410</v>
       </c>
@@ -9561,7 +9582,7 @@
         <v>287</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="135" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>410</v>
       </c>
@@ -9621,7 +9642,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="136" spans="1:20" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>410</v>
       </c>

</xml_diff>